<commit_message>
Se termina la automatizaciión, falta readme
</commit_message>
<xml_diff>
--- a/parametros/Datos.xlsx
+++ b/parametros/Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo\Downloads\KtronixScreenplay-main\aliexpressAutomation\parametros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFAE142-5F22-4D88-AA91-F8CE999A54E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22757F2F-4890-4FDB-8083-705A83E6A130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2325" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carrito" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>url</t>
   </si>
@@ -33,19 +33,10 @@
     <t>https://es.aliexpress.com/</t>
   </si>
   <si>
-    <t>producto</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>Reloj de negocios de lujo para hombre, 2 uds., calendario de acero inoxidable, relojes de esfera grande para hombre, reloj de pulsera de cuarzo informal deportivo a la moda</t>
-  </si>
-  <si>
     <t>busqueda</t>
   </si>
   <si>
-    <t>reloj hombre</t>
+    <t>Lapicero</t>
   </si>
 </sst>
 </file>
@@ -378,13 +369,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -393,13 +384,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -407,14 +392,9 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2">
-        <v>22495.439999999999</v>
-      </c>
+      <c r="D2" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>